<commit_message>
algorithm, code, and test cases
</commit_message>
<xml_diff>
--- a/test_cases.xlsx
+++ b/test_cases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zee/development/CS151_labs/PA1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caitlinburns/PycharmProjects/cs151-pa1-Ceburns/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D0D32F8-6D7A-7B45-9670-B8699C8948C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50041740-3949-5144-9F8E-57B02D802213}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="67920" windowHeight="28300" xr2:uid="{078FF010-DC04-EB46-847F-52BBCCEEE85C}"/>
+    <workbookView xWindow="820" yWindow="520" windowWidth="28800" windowHeight="16100" xr2:uid="{078FF010-DC04-EB46-847F-52BBCCEEE85C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -34,9 +34,108 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>You need to create your own tests</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="34">
+  <si>
+    <t>Path Number</t>
+  </si>
+  <si>
+    <t>in: map pieces needed</t>
+  </si>
+  <si>
+    <t>in: journey length</t>
+  </si>
+  <si>
+    <t>long</t>
+  </si>
+  <si>
+    <t>short</t>
+  </si>
+  <si>
+    <t>in: character</t>
+  </si>
+  <si>
+    <t>pirate</t>
+  </si>
+  <si>
+    <t>fairy</t>
+  </si>
+  <si>
+    <t>in: number 1-9</t>
+  </si>
+  <si>
+    <t>in: chest 1 or 2</t>
+  </si>
+  <si>
+    <t>in:rest/search</t>
+  </si>
+  <si>
+    <t>in:pocket/backpack</t>
+  </si>
+  <si>
+    <t>in:chest 1 or 2</t>
+  </si>
+  <si>
+    <t>out: days</t>
+  </si>
+  <si>
+    <t>out:pet</t>
+  </si>
+  <si>
+    <t>out:world</t>
+  </si>
+  <si>
+    <t>out:total map pieces</t>
+  </si>
+  <si>
+    <t>8 days</t>
+  </si>
+  <si>
+    <t>4 days</t>
+  </si>
+  <si>
+    <t>parrot</t>
+  </si>
+  <si>
+    <t>cat</t>
+  </si>
+  <si>
+    <t>dog</t>
+  </si>
+  <si>
+    <t>mouse</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>search</t>
+  </si>
+  <si>
+    <t>rest</t>
+  </si>
+  <si>
+    <t>pocket</t>
+  </si>
+  <si>
+    <t>backpack</t>
+  </si>
+  <si>
+    <t>enchanted forest</t>
+  </si>
+  <si>
+    <t>pirate beach</t>
+  </si>
+  <si>
+    <t>fairy castle</t>
+  </si>
+  <si>
+    <t>out: win/lose</t>
+  </si>
+  <si>
+    <t>game over</t>
+  </si>
+  <si>
+    <t>you win</t>
   </si>
 </sst>
 </file>
@@ -95,9 +194,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -135,7 +234,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -241,7 +340,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -383,7 +482,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -391,22 +490,549 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EF6E1F2-B43E-D343-BB9B-DE90F40B65C5}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.1640625" customWidth="1"/>
+    <col min="2" max="2" width="20.1640625" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" customWidth="1"/>
+    <col min="7" max="7" width="12.5" customWidth="1"/>
+    <col min="8" max="8" width="16.5" customWidth="1"/>
+    <col min="9" max="10" width="12" customWidth="1"/>
+    <col min="14" max="14" width="14.5" customWidth="1"/>
+    <col min="15" max="15" width="18.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" t="s">
+        <v>13</v>
+      </c>
+      <c r="M2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" t="s">
+        <v>15</v>
+      </c>
+      <c r="O2" t="s">
+        <v>16</v>
+      </c>
+      <c r="P2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" t="s">
+        <v>17</v>
+      </c>
+      <c r="M3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N3" t="s">
+        <v>28</v>
+      </c>
+      <c r="O3">
+        <v>4</v>
+      </c>
+      <c r="P3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M4" t="s">
+        <v>20</v>
+      </c>
+      <c r="N4" t="s">
+        <v>28</v>
+      </c>
+      <c r="O4">
+        <v>4</v>
+      </c>
+      <c r="P4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5" t="s">
+        <v>25</v>
+      </c>
+      <c r="L5" t="s">
+        <v>17</v>
+      </c>
+      <c r="M5" t="s">
+        <v>21</v>
+      </c>
+      <c r="N5" t="s">
+        <v>28</v>
+      </c>
+      <c r="O5">
+        <v>3</v>
+      </c>
+      <c r="P5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6" t="s">
+        <v>25</v>
+      </c>
+      <c r="L6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N6" t="s">
+        <v>29</v>
+      </c>
+      <c r="O6">
+        <v>3</v>
+      </c>
+      <c r="P6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7" t="s">
+        <v>25</v>
+      </c>
+      <c r="L7" t="s">
+        <v>17</v>
+      </c>
+      <c r="M7" t="s">
+        <v>19</v>
+      </c>
+      <c r="N7" t="s">
+        <v>29</v>
+      </c>
+      <c r="O7">
+        <v>4</v>
+      </c>
+      <c r="P7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8">
+        <v>6</v>
+      </c>
+      <c r="F8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8" t="s">
+        <v>24</v>
+      </c>
+      <c r="L8" t="s">
+        <v>18</v>
+      </c>
+      <c r="M8" t="s">
+        <v>20</v>
+      </c>
+      <c r="N8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O8">
+        <v>5</v>
+      </c>
+      <c r="P8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9">
+        <v>7</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9" t="s">
+        <v>24</v>
+      </c>
+      <c r="L9" t="s">
+        <v>17</v>
+      </c>
+      <c r="M9" t="s">
+        <v>21</v>
+      </c>
+      <c r="N9" t="s">
+        <v>30</v>
+      </c>
+      <c r="O9">
+        <v>6</v>
+      </c>
+      <c r="P9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10">
+        <v>8</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" t="s">
+        <v>27</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10" t="s">
+        <v>24</v>
+      </c>
+      <c r="L10" t="s">
+        <v>18</v>
+      </c>
+      <c r="M10" t="s">
+        <v>22</v>
+      </c>
+      <c r="N10" t="s">
+        <v>30</v>
+      </c>
+      <c r="O10">
+        <v>6</v>
+      </c>
+      <c r="P10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11">
+        <v>9</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="G11" t="s">
+        <v>24</v>
+      </c>
+      <c r="H11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I11">
+        <v>2</v>
+      </c>
+      <c r="J11" t="s">
+        <v>23</v>
+      </c>
+      <c r="L11" t="s">
+        <v>17</v>
+      </c>
+      <c r="M11" t="s">
+        <v>19</v>
+      </c>
+      <c r="N11" t="s">
+        <v>30</v>
+      </c>
+      <c r="O11">
+        <v>5</v>
+      </c>
+      <c r="P11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12">
+        <v>9</v>
+      </c>
+      <c r="F12">
+        <v>2</v>
+      </c>
+      <c r="G12" t="s">
+        <v>25</v>
+      </c>
+      <c r="H12" t="s">
+        <v>26</v>
+      </c>
+      <c r="I12">
+        <v>2</v>
+      </c>
+      <c r="J12" t="s">
+        <v>25</v>
+      </c>
+      <c r="L12" t="s">
+        <v>18</v>
+      </c>
+      <c r="M12" t="s">
+        <v>22</v>
+      </c>
+      <c r="N12" t="s">
+        <v>30</v>
+      </c>
+      <c r="O12">
+        <v>3</v>
+      </c>
+      <c r="P12" t="s">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>